<commit_message>
Finished to clean file R
</commit_message>
<xml_diff>
--- a/POSM_Excel_modell.xlsx
+++ b/POSM_Excel_modell.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alain/ComputerScience/Projects/R_projects/POSM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BAE0087-2136-DE45-83D9-7F23C889B288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476BFA0D-7D37-E143-81DE-B97AC92BA54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="500" windowWidth="30000" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="500" windowWidth="30000" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acerbi_model" sheetId="2" r:id="rId1"/>
-    <sheet name="compressed_model" sheetId="5" r:id="rId2"/>
+    <sheet name="compressed" sheetId="2" r:id="rId1"/>
+    <sheet name="expanded" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
@@ -24,8 +24,8 @@
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">acerbi_model!$C$2:$I$2,acerbi_model!$N$3:$N$8,acerbi_model!$Q$3:$U$8</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">compressed_model!$B$3:$AQ$3</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">compressed!$C$2:$I$2,compressed!$N$3:$N$8,compressed!$Q$3:$U$8</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">expanded!$B$3:$AQ$3</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
@@ -36,13 +36,13 @@
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">acerbi_model!$B$12</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">compressed_model!$AR$10:$AR$11</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">acerbi_model!$J$2</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">compressed_model!$AR$12:$AR$71</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">acerbi_model!$Q$3:$U$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">compressed_model!$AR$10</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">acerbi_model!$Q$3:$U$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">compressed!$B$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">expanded!$AR$10:$AR$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">compressed!$J$2</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">expanded!$AR$12:$AR$71</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">compressed!$Q$3:$U$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">expanded!$AR$10</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">compressed!$Q$3:$U$8</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
@@ -61,8 +61,8 @@
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">acerbi_model!$B$14</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">compressed_model!$AR$3</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">compressed!$B$14</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">expanded!$AR$3</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
@@ -74,13 +74,13 @@
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">acerbi_model!$B$11</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">compressed_model!$AT$10:$AT$11</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">compressed!$B$11</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">expanded!$AT$10:$AT$11</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">compressed_model!$AT$12:$AT$71</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">acerbi_model!$AC$3:$AG$8</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">compressed_model!$AT$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">acerbi_model!$W$3:$AA$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">expanded!$AT$12:$AT$71</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">compressed!$AC$3:$AG$8</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">expanded!$AT$10</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">compressed!$W$3:$AA$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
@@ -591,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -610,9 +610,7 @@
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -916,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCE5DC9-2F91-3B4A-8340-18CF43A9EAE0}">
   <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1000,7 +998,7 @@
       <c r="I2" s="7">
         <v>0</v>
       </c>
-      <c r="J2" s="23">
+      <c r="J2" s="21">
         <f>SUM(C2:I2)</f>
         <v>0.99999999999999978</v>
       </c>
@@ -1079,7 +1077,7 @@
       <c r="L3" s="13">
         <v>0.185090620379495</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="11">
         <f>SUMPRODUCT(C3:I3,$C$2:$I$2)</f>
         <v>4.9467357364243372E-3</v>
       </c>
@@ -1108,39 +1106,39 @@
       </c>
       <c r="V3" s="11"/>
       <c r="W3" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M3</f>
+        <f t="shared" ref="W3:AA8" ca="1" si="0">OFFSET($N$2,W$2,0) - $M3</f>
         <v>-4.9467357364243372E-3</v>
       </c>
       <c r="X3" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M3</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-4.9467357364243372E-3</v>
       </c>
       <c r="Y3" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M3</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.2125084523965805E-3</v>
       </c>
       <c r="Z3" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M3</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.2125084523965874E-3</v>
       </c>
       <c r="AA3" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M3</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.2125084523965996E-3</v>
       </c>
       <c r="AB3" s="11"/>
-      <c r="AC3" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="23">
+      <c r="AC3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1173,8 +1171,8 @@
       <c r="L4" s="13">
         <v>0.15083208262702799</v>
       </c>
-      <c r="M4" s="20">
-        <f t="shared" ref="M4:M8" si="0">SUMPRODUCT(C4:I4,$C$2:$I$2)</f>
+      <c r="M4" s="11">
+        <f t="shared" ref="M4:M8" si="1">SUMPRODUCT(C4:I4,$C$2:$I$2)</f>
         <v>9.1592441888209176E-3</v>
       </c>
       <c r="N4" s="9">
@@ -1202,39 +1200,39 @@
       </c>
       <c r="V4" s="11"/>
       <c r="W4" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209176E-3</v>
       </c>
       <c r="X4" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209176E-3</v>
       </c>
       <c r="Y4" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="Z4" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AA4" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1.9081958235744878E-17</v>
       </c>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="23">
+      <c r="AC4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1267,8 +1265,8 @@
       <c r="L5" s="13">
         <v>0.122914478880461</v>
       </c>
-      <c r="M5" s="20">
-        <f t="shared" si="0"/>
+      <c r="M5" s="11">
+        <f t="shared" si="1"/>
         <v>9.1592441888209229E-3</v>
       </c>
       <c r="N5" s="9">
@@ -1296,39 +1294,39 @@
       </c>
       <c r="V5" s="11"/>
       <c r="W5" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209229E-3</v>
       </c>
       <c r="X5" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209229E-3</v>
       </c>
       <c r="Y5" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="Z5" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AA5" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1.3877787807814457E-17</v>
       </c>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="23">
+      <c r="AC5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1361,8 +1359,8 @@
       <c r="L6" s="13">
         <v>0.100164161730854</v>
       </c>
-      <c r="M6" s="20">
-        <f t="shared" si="0"/>
+      <c r="M6" s="11">
+        <f t="shared" si="1"/>
         <v>9.1592441888209176E-3</v>
       </c>
       <c r="N6" s="9">
@@ -1390,39 +1388,39 @@
       </c>
       <c r="V6" s="11"/>
       <c r="W6" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209176E-3</v>
       </c>
       <c r="X6" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-9.1592441888209176E-3</v>
       </c>
       <c r="Y6" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="Z6" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="AA6" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1.9081958235744878E-17</v>
       </c>
       <c r="AB6" s="11"/>
-      <c r="AC6" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="23">
+      <c r="AC6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1455,8 +1453,8 @@
       <c r="L7" s="13">
         <v>8.1624714896298106E-2</v>
       </c>
-      <c r="M7" s="20">
-        <f t="shared" si="0"/>
+      <c r="M7" s="11">
+        <f t="shared" si="1"/>
         <v>-7.9866791601973811E-2</v>
       </c>
       <c r="N7" s="9">
@@ -1484,39 +1482,39 @@
       </c>
       <c r="V7" s="11"/>
       <c r="W7" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.9866791601973811E-2</v>
       </c>
       <c r="X7" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.9866791601973811E-2</v>
       </c>
       <c r="Y7" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8.9026035790794725E-2</v>
       </c>
       <c r="Z7" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8.9026035790794739E-2</v>
       </c>
       <c r="AA7" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8.9026035790794752E-2</v>
       </c>
       <c r="AB7" s="11"/>
-      <c r="AC7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="23">
+      <c r="AC7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1549,14 +1547,14 @@
       <c r="L8" s="13">
         <v>6.6516745777842903E-2</v>
       </c>
-      <c r="M8" s="20">
-        <f t="shared" si="0"/>
+      <c r="M8" s="11">
+        <f t="shared" si="1"/>
         <v>-5.5767670091329876E-4</v>
       </c>
       <c r="N8" s="9">
         <v>0</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="19">
         <f ca="1">SUM(O3:O7)</f>
         <v>8.8106936602694846E-3</v>
       </c>
@@ -1578,39 +1576,39 @@
       </c>
       <c r="V8" s="11"/>
       <c r="W8" s="12">
-        <f ca="1">OFFSET($N$2,W$2,0) - $M8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5.5767670091329876E-4</v>
       </c>
       <c r="X8" s="12">
-        <f ca="1">OFFSET($N$2,X$2,0) - $M8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5.5767670091329876E-4</v>
       </c>
       <c r="Y8" s="12">
-        <f ca="1">OFFSET($N$2,Y$2,0) - $M8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.7169208897342173E-3</v>
       </c>
       <c r="Z8" s="12">
-        <f ca="1">OFFSET($N$2,Z$2,0) - $M8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.7169208897342242E-3</v>
       </c>
       <c r="AA8" s="12">
-        <f ca="1">OFFSET($N$2,AA$2,0) - $M8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.7169208897342346E-3</v>
       </c>
       <c r="AB8" s="11"/>
-      <c r="AC8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="23">
+      <c r="AC8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1618,36 +1616,36 @@
       <c r="B9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <f>AVERAGE(C3:C8)</f>
         <v>-1.1650410843356907E-2</v>
       </c>
-      <c r="D9" s="22">
-        <f t="shared" ref="D9:I9" si="1">AVERAGE(D3:D8)</f>
+      <c r="D9" s="20">
+        <f t="shared" ref="D9:I9" si="2">AVERAGE(D3:D8)</f>
         <v>-1.062030765206462E-2</v>
       </c>
-      <c r="E9" s="22">
-        <f t="shared" si="1"/>
+      <c r="E9" s="20">
+        <f t="shared" si="2"/>
         <v>-1.3043193613093251E-2</v>
       </c>
-      <c r="F9" s="22">
-        <f t="shared" si="1"/>
+      <c r="F9" s="20">
+        <f t="shared" si="2"/>
         <v>-6.2329739784453145E-3</v>
       </c>
-      <c r="G9" s="22">
-        <f t="shared" si="1"/>
+      <c r="G9" s="20">
+        <f t="shared" si="2"/>
         <v>-6.5862216033286515E-3</v>
       </c>
-      <c r="H9" s="22">
-        <f t="shared" si="1"/>
+      <c r="H9" s="20">
+        <f t="shared" si="2"/>
         <v>-1.9139067991811601E-2</v>
       </c>
-      <c r="I9" s="22">
-        <f t="shared" si="1"/>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
         <v>-8.9670643812791492E-3</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="M9" s="21">
+      <c r="M9" s="19">
         <f>SUM(M3:M8)</f>
         <v>-4.8000000000000015E-2</v>
       </c>
@@ -1656,23 +1654,23 @@
       <c r="P9" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="19">
         <f>SUM(Q3:Q8)</f>
         <v>8.0424468302887103E-2</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="19">
         <f>SUM(R3:R8)</f>
         <v>8.0424468302887117E-2</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="19">
         <f>SUM(S3:S8)</f>
         <v>0.10295546513292556</v>
       </c>
-      <c r="T9" s="21">
+      <c r="T9" s="19">
         <f>SUM(T3:T8)</f>
         <v>0.10295546513292557</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="19">
         <f>SUM(U3:U8)</f>
         <v>0.10295546513292562</v>
       </c>
@@ -1685,7 +1683,7 @@
       <c r="AB9" s="11"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="11">
@@ -1701,10 +1699,10 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="D12" s="1"/>
@@ -1721,7 +1719,7 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="17">
@@ -1739,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248C0EA1-0E33-194E-AD2B-FBBE605E73B0}">
   <dimension ref="A1:AT71"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2166,7 +2164,7 @@
         <v>3.5787596509385716E-3</v>
       </c>
       <c r="I4" s="11" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">SUMPRODUCT(I5,I6,I7)</f>
         <v>#REF!</v>
       </c>
       <c r="J4" s="11" t="e">
@@ -2463,23 +2461,23 @@
         <v>6.6516745777842903E-2</v>
       </c>
       <c r="I6" s="11" t="e">
-        <f ca="1">OFFSET(#REF!, compressed_model!B1, 0)</f>
+        <f ca="1">OFFSET(#REF!, expanded!B1, 0)</f>
         <v>#REF!</v>
       </c>
       <c r="J6" s="11" t="e">
-        <f ca="1">OFFSET(#REF!, compressed_model!C1, 0)</f>
+        <f ca="1">OFFSET(#REF!, expanded!C1, 0)</f>
         <v>#REF!</v>
       </c>
       <c r="K6" s="11" t="e">
-        <f ca="1">OFFSET(#REF!, compressed_model!D1, 0)</f>
+        <f ca="1">OFFSET(#REF!, expanded!D1, 0)</f>
         <v>#REF!</v>
       </c>
       <c r="L6" s="11" t="e">
-        <f ca="1">OFFSET(#REF!, compressed_model!E1, 0)</f>
+        <f ca="1">OFFSET(#REF!, expanded!E1, 0)</f>
         <v>#REF!</v>
       </c>
       <c r="M6" s="11" t="e">
-        <f ca="1">OFFSET(#REF!, compressed_model!F1, 0)</f>
+        <f ca="1">OFFSET(#REF!, expanded!F1, 0)</f>
         <v>#REF!</v>
       </c>
       <c r="N6" s="11" t="e">

</xml_diff>